<commit_message>
Se actualiza planilla con los datos de la reserva Se actualizan asistentes teniendo en cuenta que asisten "TODOS" de Crescentini. Se ajustan cantidades a comprar. Se actualiza presupuesto total.
</commit_message>
<xml_diff>
--- a/Documentacion/Documentos de Gestión/Presentación comercial/Catering.xlsx
+++ b/Documentacion/Documentos de Gestión/Presentación comercial/Catering.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="105" windowWidth="14115" windowHeight="4695"/>
@@ -11,12 +11,12 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
   <si>
     <t>Descripción</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Sandwiches de miga</t>
   </si>
   <si>
-    <t>Precio total estimado</t>
-  </si>
-  <si>
     <t>Cantidad promedio por persona (calc)</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
     <t>Pasta frola o similar</t>
   </si>
   <si>
-    <t>Coca cola 2,5l</t>
-  </si>
-  <si>
-    <t>Sprite 2,5l</t>
-  </si>
-  <si>
     <t>Botellas agua</t>
   </si>
   <si>
@@ -105,12 +96,6 @@
     <t>Leche en polvo</t>
   </si>
   <si>
-    <t>1 vaso</t>
-  </si>
-  <si>
-    <t>Precio final real</t>
-  </si>
-  <si>
     <t>1 caja</t>
   </si>
   <si>
@@ -142,13 +127,47 @@
   </si>
   <si>
     <t>Total estimado</t>
+  </si>
+  <si>
+    <t>Reservado</t>
+  </si>
+  <si>
+    <t>Reservado bajo número de cliente 1134228821 para el jueves 11 desde las 17hs.
+Retirar en Estado de Israel 4102</t>
+  </si>
+  <si>
+    <t>Coca cola 2,25l</t>
+  </si>
+  <si>
+    <t>Sprite 2,25l</t>
+  </si>
+  <si>
+    <t>Coca cola light 2,25l</t>
+  </si>
+  <si>
+    <t>Sprite zero 2,25l</t>
+  </si>
+  <si>
+    <t>Gonzalo</t>
+  </si>
+  <si>
+    <t>Precio total (estimado)</t>
+  </si>
+  <si>
+    <t>0,5 lts</t>
+  </si>
+  <si>
+    <t>0,75 (porción)</t>
+  </si>
+  <si>
+    <t>Presupuesto total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,7 +176,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -176,14 +195,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -206,11 +219,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -237,12 +287,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -333,7 +392,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -368,7 +426,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -544,32 +601,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:M27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A2:L30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="3.85546875" customWidth="1"/>
     <col min="2" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="16.28515625" customWidth="1"/>
     <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="17.85546875" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="9" width="13.7109375" customWidth="1"/>
-    <col min="10" max="10" width="13.5703125" customWidth="1"/>
-    <col min="12" max="12" width="26.5703125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="8" width="13.7109375" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="11" max="11" width="26.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="30">
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="5">
-        <v>36</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
@@ -577,9 +634,8 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -592,9 +648,8 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="1:13" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" ht="39.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="6" t="s">
         <v>0</v>
@@ -603,607 +658,668 @@
         <v>1</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>32</v>
       </c>
       <c r="J4" s="7" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="K4" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="M4" s="1"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+      <c r="L4" s="1"/>
+    </row>
+    <row r="5" spans="1:12" ht="75">
       <c r="A5" s="1"/>
       <c r="B5" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="2">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D5" s="2">
         <f>C5/$C$2</f>
-        <v>2</v>
-      </c>
-      <c r="E5" s="2">
-        <v>250</v>
+        <v>2.4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J5" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J5" s="2">
+        <v>300</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K5" s="2"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="1"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L5" s="1"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="1"/>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="2">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D6" s="2">
         <f>C6/$C$2</f>
-        <v>1</v>
-      </c>
-      <c r="E6" s="2">
-        <v>100</v>
+        <v>0.75</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K6" s="2"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="1"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J6" s="2">
+        <v>120</v>
+      </c>
+      <c r="K6" s="4"/>
+      <c r="L6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="75">
       <c r="A7" s="1"/>
       <c r="B7" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C7" s="2">
         <v>3</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="2">
-        <v>180</v>
+        <v>46</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>7</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="J7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="J7" s="2">
+        <v>180</v>
+      </c>
+      <c r="K7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="2"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="1"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L7" s="1"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="1"/>
       <c r="B8" s="4" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="C8" s="2">
-        <v>3</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="2">
+        <v>2</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>45</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K8" s="2"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="1"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J8" s="2">
+        <v>40</v>
+      </c>
+      <c r="K8" s="4"/>
+      <c r="L8" s="1"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="1"/>
       <c r="B9" s="4" t="s">
-        <v>19</v>
+        <v>41</v>
       </c>
       <c r="C9" s="2">
-        <v>3</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="2">
-        <v>45</v>
+        <v>2</v>
+      </c>
+      <c r="D9" s="14"/>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K9" s="2"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="1"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J9" s="2">
+        <v>40</v>
+      </c>
+      <c r="K9" s="4"/>
+      <c r="L9" s="1"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="1"/>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C10" s="2">
-        <v>2</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="2">
-        <v>20</v>
+        <v>1</v>
+      </c>
+      <c r="D10" s="14"/>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10" s="2"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="1"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J10" s="2">
+        <v>20</v>
+      </c>
+      <c r="K10" s="4"/>
+      <c r="L10" s="1"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" s="1"/>
       <c r="B11" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E11" s="2">
-        <v>25</v>
+        <v>42</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="14"/>
+      <c r="E11" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11" s="2"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="1"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J11" s="2">
+        <v>20</v>
+      </c>
+      <c r="K11" s="4"/>
+      <c r="L11" s="1"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="1"/>
       <c r="B12" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D12" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>20</v>
+        <v>17</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K12" s="2"/>
-      <c r="L12" s="4"/>
-      <c r="M12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J12" s="2">
+        <v>20</v>
+      </c>
+      <c r="K12" s="4"/>
+      <c r="L12" s="1"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="1"/>
       <c r="B13" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="2">
-        <v>50</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1.5</v>
-      </c>
-      <c r="E13" s="2">
-        <v>20</v>
+        <v>23</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K13" s="2"/>
-      <c r="L13" s="4"/>
-      <c r="M13" s="1"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J13" s="2">
+        <v>25</v>
+      </c>
+      <c r="K13" s="4"/>
+      <c r="L13" s="1"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1"/>
       <c r="B14" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C14" s="2">
-        <v>50</v>
+        <v>22</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E14" s="2">
-        <v>40</v>
+        <v>13</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K14" s="2"/>
-      <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J14" s="2">
+        <v>20</v>
+      </c>
+      <c r="K14" s="4"/>
+      <c r="L14" s="1"/>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" s="1"/>
       <c r="B15" s="4" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2">
-        <v>10</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="2">
-        <v>15</v>
+        <v>50</v>
+      </c>
+      <c r="D15" s="2">
+        <v>1.5</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>12</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K15" s="2"/>
-      <c r="L15" s="4"/>
-      <c r="M15" s="1"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
-      <c r="B16" s="8"/>
-      <c r="C16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="9"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="8"/>
-      <c r="M16" s="1"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+      <c r="J15" s="2">
+        <v>20</v>
+      </c>
+      <c r="K15" s="4"/>
+      <c r="L15" s="1"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="B16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="2">
+        <v>50</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J16" s="2">
+        <v>40</v>
+      </c>
+      <c r="K16" s="3"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="1"/>
       <c r="B17" s="4" t="s">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="C17" s="2">
-        <f>SUM(E5:E15)</f>
-        <v>760</v>
-      </c>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="9"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="L17" s="8"/>
-      <c r="M17" s="1"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J17" s="2">
+        <v>20</v>
+      </c>
+      <c r="K17" s="4"/>
+      <c r="L17" s="1"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="1"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="8"/>
       <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="1"/>
       <c r="B19" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K19" s="2"/>
-      <c r="L19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M19" s="1"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2">
+        <f>SUM(J5:J17)</f>
+        <v>865</v>
+      </c>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="1"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="1"/>
       <c r="B20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K20" s="2"/>
-      <c r="L20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" s="1"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+        <v>47</v>
+      </c>
+      <c r="C20" s="2">
+        <v>900</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="1"/>
+    </row>
+    <row r="21" spans="1:12">
       <c r="A21" s="1"/>
-      <c r="B21" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K21" s="2"/>
-      <c r="L21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M21" s="1"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+    </row>
+    <row r="22" spans="1:12">
       <c r="A22" s="1"/>
-      <c r="B22" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="11"/>
-      <c r="H22" s="12"/>
-      <c r="I22" s="12"/>
-      <c r="J22" s="12" t="s">
-        <v>38</v>
-      </c>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="1"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="2"/>
+      <c r="K22" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L22" s="1"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="1"/>
-      <c r="B23" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K23" s="4"/>
-      <c r="L23" s="4"/>
-      <c r="M23" s="1"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B23" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J23" s="2"/>
+      <c r="K23" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L23" s="1"/>
+    </row>
+    <row r="24" spans="1:12">
       <c r="A24" s="1"/>
       <c r="B24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
-      <c r="H24" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="4"/>
-      <c r="J24" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="K24" s="4"/>
-      <c r="L24" s="4"/>
-      <c r="M24" s="1"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J24" s="2"/>
+      <c r="K24" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L24" s="1"/>
+    </row>
+    <row r="25" spans="1:12">
       <c r="A25" s="1"/>
+      <c r="B25" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="H25" s="12"/>
+      <c r="I25" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
       <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:12">
       <c r="A26" s="1"/>
+      <c r="B26" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J26" s="4"/>
+      <c r="K26" s="4"/>
       <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:12">
       <c r="A27" s="1"/>
+      <c r="B27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D8:D12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>